<commit_message>
Changed Attach and Support document names.
</commit_message>
<xml_diff>
--- a/Fulcrum_PreProd_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/Generic_Data.xlsx
+++ b/Fulcrum_PreProd_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/Generic_Data.xlsx
@@ -10,7 +10,7 @@
     <sheet name="user_credentials" sheetId="1" r:id="rId1"/>
     <sheet name="DocumentDetails" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -89,9 +89,6 @@
     <t>Register</t>
   </si>
   <si>
-    <t>Test 1 ta.docx</t>
-  </si>
-  <si>
     <t>Attach Document</t>
   </si>
   <si>
@@ -102,12 +99,15 @@
   </si>
   <si>
     <t>BrowseDocument.docx</t>
+  </si>
+  <si>
+    <t>ATCRL-AOT-ACV-BIM-002436.docx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -578,7 +578,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -604,26 +606,26 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
         <v>27</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>